<commit_message>
changes - first clear
</commit_message>
<xml_diff>
--- a/analysis/files/support/wide_format_for_covid.xlsx
+++ b/analysis/files/support/wide_format_for_covid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ni3054ch\Work Folders\Documents\reloc_age_analysis\analysis\files\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBEC2AB1-DCA8-4FD3-BCBB-E2E385411F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DF5DA5-CBA0-447A-8951-5D41E3836533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9313AC2E-894D-40D5-B4B3-EEF320B1BAE0}"/>
+    <workbookView xWindow="705" yWindow="17325" windowWidth="21600" windowHeight="11325" xr2:uid="{9313AC2E-894D-40D5-B4B3-EEF320B1BAE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>lopnr</t>
   </si>
@@ -159,6 +159,63 @@
   </si>
   <si>
     <t>total_number_stays_2015_2019?</t>
+  </si>
+  <si>
+    <t>group by , sum flu risk</t>
+  </si>
+  <si>
+    <t>icd</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>J21</t>
+  </si>
+  <si>
+    <t>flu_risk?</t>
+  </si>
+  <si>
+    <t>J20</t>
+  </si>
+  <si>
+    <t>flu_risk_cat</t>
+  </si>
+  <si>
+    <t>Anemia</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lung </t>
+  </si>
+  <si>
+    <t>H20</t>
+  </si>
+  <si>
+    <t>243j</t>
+  </si>
+  <si>
+    <t>flu_risk ever?</t>
+  </si>
+  <si>
+    <t>flu_risk_last 3</t>
+  </si>
+  <si>
+    <t>flu_risk_last 5</t>
+  </si>
+  <si>
+    <t>U71?</t>
+  </si>
+  <si>
+    <t>U72?</t>
+  </si>
+  <si>
+    <t>U71|U72</t>
   </si>
 </sst>
 </file>
@@ -200,8 +257,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,20 +574,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A47D0D3-2938-48F5-826D-2591BB6B3F2C}">
-  <dimension ref="D4:AR5"/>
+  <dimension ref="D4:AR27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AR6" sqref="AR6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="25" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22" customWidth="1"/>
+    <col min="17" max="17" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="25" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="36" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -788,6 +847,201 @@
         <v>50</v>
       </c>
     </row>
+    <row r="12" spans="4:44" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" t="s">
+        <v>54</v>
+      </c>
+      <c r="J23" t="s">
+        <v>55</v>
+      </c>
+      <c r="K23" t="s">
+        <v>56</v>
+      </c>
+      <c r="L23" t="s">
+        <v>57</v>
+      </c>
+      <c r="M23" t="s">
+        <v>58</v>
+      </c>
+      <c r="N23" t="s">
+        <v>59</v>
+      </c>
+      <c r="O23" t="s">
+        <v>38</v>
+      </c>
+      <c r="P23" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>12</v>
+      </c>
+      <c r="E24">
+        <v>2000</v>
+      </c>
+      <c r="F24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>100</v>
+      </c>
+      <c r="Q24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>12</v>
+      </c>
+      <c r="E25">
+        <v>2001</v>
+      </c>
+      <c r="F25" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>12</v>
+      </c>
+      <c r="E26">
+        <v>2002</v>
+      </c>
+      <c r="F26" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>12</v>
+      </c>
+      <c r="E27">
+        <v>2003</v>
+      </c>
+      <c r="F27" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>